<commit_message>
intermediate revision - adding insertion new columns
</commit_message>
<xml_diff>
--- a/fillo_examples/src/test/resources/StatesData.xlsx
+++ b/fillo_examples/src/test/resources/StatesData.xlsx
@@ -2,17 +2,17 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" date1904="false" showObjects="all"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="States" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="States" r:id="rId2" sheetId="1" state="visible"/>
+    <sheet name="Sheet2" r:id="rId3" sheetId="2" state="visible"/>
+    <sheet name="Sheet3" r:id="rId4" sheetId="3" state="visible"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr iterate="false" iterateCount="100" iterateDelta="0.0001" refMode="A1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="24">
   <si>
     <t xml:space="preserve">Sno</t>
   </si>
@@ -79,6 +79,21 @@
   </si>
   <si>
     <t xml:space="preserve">Lucknow</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Rajastan</t>
+  </si>
+  <si>
+    <t>Jaipur</t>
+  </si>
+  <si>
+    <t>North</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
   </si>
 </sst>
 </file>
@@ -135,14 +150,14 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
@@ -151,55 +166,55 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" name="Comma" xfId="15"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="16"/>
+    <cellStyle builtinId="4" name="Currency" xfId="17"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="18"/>
+    <cellStyle builtinId="5" name="Percent" xfId="19"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -269,22 +284,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9:D22"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A9" activeCellId="0" pane="topLeft" sqref="A9:D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.54"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="8.54" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="15.15" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="11.29" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="7.15" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="1025" customWidth="true" hidden="false" style="0" width="8.54" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -298,7 +313,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="2">
       <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
@@ -306,13 +321,13 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
       <c r="A3" s="2" t="n">
         <v>2</v>
       </c>
@@ -326,7 +341,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="4">
       <c r="A4" s="2" t="n">
         <v>3</v>
       </c>
@@ -340,7 +355,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
       <c r="A5" s="2" t="n">
         <v>4</v>
       </c>
@@ -354,7 +369,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="6">
       <c r="A6" s="2" t="n">
         <v>5</v>
       </c>
@@ -368,7 +383,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="7">
       <c r="A7" s="3" t="n">
         <v>6</v>
       </c>
@@ -382,7 +397,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="8">
       <c r="A8" s="3" t="n">
         <v>7</v>
       </c>
@@ -396,24 +411,178 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="9">
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="10">
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="11">
+      <c r="A11"/>
+      <c r="B11"/>
+      <c r="C11"/>
+      <c r="D11"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="12">
+      <c r="A12"/>
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="D12"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="13">
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="14">
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="15">
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="16">
+      <c r="A16"/>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="17">
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="18">
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="19">
+      <c r="A19"/>
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="20">
+      <c r="A20"/>
+      <c r="B20"/>
+      <c r="C20"/>
+      <c r="D20"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="21">
+      <c r="A21"/>
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="22">
+      <c r="A22"/>
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -428,18 +597,18 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A9:D22 A1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="A9:D22 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.54"/>
+    <col min="1" max="1025" customWidth="true" hidden="false" style="0" width="8.54" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -454,18 +623,18 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A9:D22 A1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="A9:D22 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.54"/>
+    <col min="1" max="1025" customWidth="true" hidden="false" style="0" width="8.54" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>